<commit_message>
Add comments inside the code
</commit_message>
<xml_diff>
--- a/cea/databases/CH/assemblies/ENVELOPE.xlsx
+++ b/cea/databases/CH/assemblies/ENVELOPE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luis.santos\Documents\CityEnergyAnalyst\CityEnergyAnalyst\cea\databases\CH\assemblies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmeshkin\Documents\GitHub\CityEnergyAnalyst\cea\databases\CH\assemblies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F82EFC04-C9C2-44FD-BADA-266BC6D030ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2289653A-A5B2-435C-AFAE-CB2A3E3F5DF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="18360" windowHeight="10320" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONSTRUCTION" sheetId="7" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="114">
   <si>
     <t>Description</t>
   </si>
@@ -361,16 +361,34 @@
   </si>
   <si>
     <t>FLOOR_AS6</t>
+  </si>
+  <si>
+    <t>Service_Life_WIN</t>
+  </si>
+  <si>
+    <t>Service_Life_ROOF</t>
+  </si>
+  <si>
+    <t>Service_Life_WALL</t>
+  </si>
+  <si>
+    <t>Service_Life_FLOOR</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>Service life reference : https://doi.org/10.1016/j.dib.2021.107062</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="187" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -396,6 +414,25 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF8C8C8C"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="4">
@@ -457,7 +494,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -480,7 +517,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="187" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -493,10 +530,34 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2 2" xfId="1"/>
+    <cellStyle name="Normal 2 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -773,21 +834,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="22.453125" customWidth="1"/>
     <col min="2" max="2" width="19.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -798,7 +859,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3">
       <c r="A2" s="9" t="s">
         <v>37</v>
       </c>
@@ -809,7 +870,7 @@
         <v>110000</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3">
       <c r="A3" s="9" t="s">
         <v>38</v>
       </c>
@@ -820,7 +881,7 @@
         <v>165000</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3">
       <c r="A4" s="9" t="s">
         <v>36</v>
       </c>
@@ -837,20 +898,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="17.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -861,7 +922,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3">
       <c r="A2" s="9" t="s">
         <v>43</v>
       </c>
@@ -872,7 +933,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3">
       <c r="A3" s="9" t="s">
         <v>39</v>
       </c>
@@ -883,7 +944,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3">
       <c r="A4" s="9" t="s">
         <v>44</v>
       </c>
@@ -894,7 +955,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3">
       <c r="A5" s="9" t="s">
         <v>42</v>
       </c>
@@ -905,7 +966,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3">
       <c r="A6" s="9" t="s">
         <v>40</v>
       </c>
@@ -916,7 +977,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3">
       <c r="A7" s="9" t="s">
         <v>41</v>
       </c>
@@ -933,14 +994,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="I1" sqref="I1:I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="51.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
@@ -948,9 +1009,10 @@
     <col min="4" max="4" width="8.7265625" customWidth="1"/>
     <col min="5" max="6" width="7.81640625" customWidth="1"/>
     <col min="7" max="7" width="19.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -972,8 +1034,14 @@
       <c r="G1" s="11" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H1" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="10" t="s">
         <v>5</v>
       </c>
@@ -995,8 +1063,14 @@
       <c r="G2" s="12">
         <v>47</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H2" s="4">
+        <v>30</v>
+      </c>
+      <c r="I2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="10" t="s">
         <v>31</v>
       </c>
@@ -1018,8 +1092,11 @@
       <c r="G3" s="12">
         <v>62</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H3" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="10" t="s">
         <v>30</v>
       </c>
@@ -1041,8 +1118,11 @@
       <c r="G4" s="12">
         <v>69</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H4" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="10" t="s">
         <v>6</v>
       </c>
@@ -1064,8 +1144,11 @@
       <c r="G5" s="12">
         <v>123</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H5" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="10" t="s">
         <v>46</v>
       </c>
@@ -1087,8 +1170,11 @@
       <c r="G6" s="12">
         <v>123</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H6" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="10" t="s">
         <v>7</v>
       </c>
@@ -1110,8 +1196,11 @@
       <c r="G7" s="12">
         <v>123</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H7" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="10" t="s">
         <v>8</v>
       </c>
@@ -1133,8 +1222,11 @@
       <c r="G8" s="12">
         <v>70</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H8" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="10" t="s">
         <v>49</v>
       </c>
@@ -1156,8 +1248,11 @@
       <c r="G9" s="12">
         <v>47</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H9" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="10" t="s">
         <v>50</v>
       </c>
@@ -1179,8 +1274,11 @@
       <c r="G10" s="12">
         <v>62</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H10" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="10" t="s">
         <v>51</v>
       </c>
@@ -1202,21 +1300,25 @@
       <c r="G11" s="12">
         <v>62</v>
       </c>
+      <c r="H11" s="4">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="I1" sqref="I1:I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="54.81640625" customWidth="1"/>
     <col min="2" max="2" width="10.26953125" bestFit="1" customWidth="1"/>
@@ -1224,9 +1326,10 @@
     <col min="4" max="4" width="10.1796875" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
     <col min="7" max="7" width="20.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1248,8 +1351,14 @@
       <c r="G1" s="11" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H1" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="10" t="s">
         <v>21</v>
       </c>
@@ -1272,8 +1381,14 @@
       <c r="G2" s="12">
         <v>112</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H2" s="4">
+        <v>30</v>
+      </c>
+      <c r="I2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="10" t="s">
         <v>20</v>
       </c>
@@ -1296,8 +1411,11 @@
       <c r="G3" s="12">
         <v>112</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H3" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="10" t="s">
         <v>23</v>
       </c>
@@ -1320,8 +1438,11 @@
       <c r="G4" s="12">
         <v>112</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H4" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="10" t="s">
         <v>22</v>
       </c>
@@ -1344,8 +1465,11 @@
       <c r="G5" s="12">
         <v>112</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H5" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="10" t="s">
         <v>24</v>
       </c>
@@ -1368,8 +1492,11 @@
       <c r="G6" s="12">
         <v>113</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H6" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="10" t="s">
         <v>25</v>
       </c>
@@ -1392,8 +1519,11 @@
       <c r="G7" s="12">
         <v>113</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H7" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="10" t="s">
         <v>47</v>
       </c>
@@ -1416,28 +1546,34 @@
       <c r="G8" s="12">
         <v>112</v>
       </c>
+      <c r="H8" s="4">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="I1" sqref="I1:I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="48.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.453125" customWidth="1"/>
-    <col min="7" max="7" width="20.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.26953125" style="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1456,11 +1592,17 @@
       <c r="F1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="19" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H1" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="3" t="s">
         <v>32</v>
       </c>
@@ -1480,11 +1622,17 @@
         <f t="shared" ref="F2:F8" si="0">1-D2</f>
         <v>0.31999999999999995</v>
       </c>
-      <c r="G2" s="12">
+      <c r="G2" s="17">
         <v>57</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H2" s="6">
+        <v>38</v>
+      </c>
+      <c r="I2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="3" t="s">
         <v>29</v>
       </c>
@@ -1504,11 +1652,14 @@
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="17">
         <v>112</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H3" s="6">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="3" t="s">
         <v>28</v>
       </c>
@@ -1528,11 +1679,14 @@
         <f t="shared" si="0"/>
         <v>0.7</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="17">
         <v>112</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H4" s="6">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="3" t="s">
         <v>26</v>
       </c>
@@ -1552,11 +1706,14 @@
         <f t="shared" si="0"/>
         <v>0.35</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="17">
         <v>112</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H5" s="6">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="3" t="s">
         <v>27</v>
       </c>
@@ -1576,11 +1733,14 @@
         <f t="shared" si="0"/>
         <v>0.15000000000000002</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="17">
         <v>112</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H6" s="6">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="3" t="s">
         <v>48</v>
       </c>
@@ -1600,11 +1760,14 @@
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="17">
         <v>112</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H7" s="6">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="3" t="s">
         <v>97</v>
       </c>
@@ -1624,11 +1787,14 @@
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="17">
         <v>34</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H8" s="6">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="3" t="s">
         <v>94</v>
       </c>
@@ -1648,32 +1814,41 @@
         <f>1-D9</f>
         <v>0.4</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G9" s="17">
         <v>73</v>
       </c>
+      <c r="H9" s="6">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="20"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="48.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.7265625" customWidth="1"/>
     <col min="3" max="3" width="10.453125" customWidth="1"/>
     <col min="4" max="4" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1686,8 +1861,14 @@
       <c r="D1" s="11" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E1" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="3" t="s">
         <v>100</v>
       </c>
@@ -1700,8 +1881,14 @@
       <c r="D2" s="12">
         <v>113</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E2" s="4">
+        <v>74</v>
+      </c>
+      <c r="F2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="3" t="s">
         <v>98</v>
       </c>
@@ -1715,8 +1902,11 @@
         <f>D2+44</f>
         <v>157</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E3" s="4">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="3" t="s">
         <v>101</v>
       </c>
@@ -1729,8 +1919,11 @@
       <c r="D4" s="12">
         <v>180</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E4" s="4">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="3" t="s">
         <v>103</v>
       </c>
@@ -1744,8 +1937,11 @@
         <f>D2+135</f>
         <v>248</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E5" s="4">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="3" t="s">
         <v>104</v>
       </c>
@@ -1759,8 +1955,11 @@
         <f>D3+135</f>
         <v>292</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E6" s="4">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="3" t="s">
         <v>105</v>
       </c>
@@ -1774,27 +1973,36 @@
         <f>D4+135</f>
         <v>315</v>
       </c>
+      <c r="E7" s="4">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="16"/>
+      <c r="B8" s="15"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="45.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1806,7 +2014,7 @@
       </c>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1818,7 +2026,7 @@
       </c>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
@@ -1830,7 +2038,7 @@
       </c>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
some formatting adjustments for consistency
</commit_message>
<xml_diff>
--- a/cea/databases/CH/assemblies/ENVELOPE.xlsx
+++ b/cea/databases/CH/assemblies/ENVELOPE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmeshkin\Documents\GitHub\CityEnergyAnalyst\cea\databases\CH\assemblies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinmo/Documents/Projects/PV/CEA case studies/dummy/inputs/technology/assemblies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2289653A-A5B2-435C-AFAE-CB2A3E3F5DF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF88A1EE-B6AB-144A-864E-3ADAA09C3669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="18360" windowHeight="10320" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONSTRUCTION" sheetId="7" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="114">
   <si>
     <t>Description</t>
   </si>
@@ -388,7 +388,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -416,13 +416,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -433,6 +426,7 @@
       <sz val="10"/>
       <color rgb="FF8C8C8C"/>
       <name val="Arial Unicode MS"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -494,12 +488,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -511,38 +505,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -551,7 +529,7 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -837,18 +815,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.453125" customWidth="1"/>
-    <col min="2" max="2" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.5" customWidth="1"/>
+    <col min="2" max="2" width="19.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -859,8 +837,8 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
         <v>37</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -870,8 +848,8 @@
         <v>110000</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
         <v>38</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -881,8 +859,8 @@
         <v>165000</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
         <v>36</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -902,16 +880,16 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.26953125" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -922,8 +900,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
         <v>43</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -933,8 +911,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
         <v>39</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -944,8 +922,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
         <v>44</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -955,8 +933,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="9" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
         <v>42</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -966,8 +944,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
         <v>40</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -977,8 +955,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
         <v>41</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -998,21 +976,22 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I2"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="51.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.453125" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" customWidth="1"/>
-    <col min="5" max="6" width="7.81640625" customWidth="1"/>
-    <col min="7" max="7" width="19.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" customWidth="1"/>
+    <col min="5" max="6" width="7.83203125" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="52.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1031,18 +1010,18 @@
       <c r="F1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="9" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -1060,18 +1039,18 @@
       <c r="F2" s="5">
         <v>0.2</v>
       </c>
-      <c r="G2" s="12">
+      <c r="G2" s="6">
         <v>47</v>
       </c>
       <c r="H2" s="4">
         <v>30</v>
       </c>
-      <c r="I2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="10" t="s">
+      <c r="I2" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
         <v>31</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -1089,15 +1068,18 @@
       <c r="F3" s="5">
         <v>0.2</v>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="6">
         <v>62</v>
       </c>
       <c r="H3" s="4">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="10" t="s">
+      <c r="I3" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
         <v>30</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -1115,15 +1097,18 @@
       <c r="F4" s="5">
         <v>0.2</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="6">
         <v>69</v>
       </c>
       <c r="H4" s="4">
         <v>30</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="10" t="s">
+      <c r="I4" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -1141,15 +1126,18 @@
       <c r="F5" s="5">
         <v>0.2</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="6">
         <v>123</v>
       </c>
       <c r="H5" s="4">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="10" t="s">
+      <c r="I5" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
         <v>46</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -1158,7 +1146,7 @@
       <c r="C6" s="4">
         <v>0.99</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="4">
         <v>0.7</v>
       </c>
       <c r="E6" s="5">
@@ -1167,15 +1155,18 @@
       <c r="F6" s="5">
         <v>0.2</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="6">
         <v>123</v>
       </c>
       <c r="H6" s="4">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="10" t="s">
+      <c r="I6" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -1193,15 +1184,18 @@
       <c r="F7" s="5">
         <v>0.2</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="6">
         <v>123</v>
       </c>
       <c r="H7" s="4">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="10" t="s">
+      <c r="I7" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -1219,15 +1213,18 @@
       <c r="F8" s="5">
         <v>0.2</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="6">
         <v>70</v>
       </c>
       <c r="H8" s="4">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="10" t="s">
+      <c r="I8" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
         <v>49</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -1245,15 +1242,18 @@
       <c r="F9" s="5">
         <v>0.2</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G9" s="6">
         <v>47</v>
       </c>
       <c r="H9" s="4">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="10" t="s">
+      <c r="I9" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
         <v>50</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -1271,15 +1271,18 @@
       <c r="F10" s="5">
         <v>0.2</v>
       </c>
-      <c r="G10" s="12">
+      <c r="G10" s="6">
         <v>62</v>
       </c>
       <c r="H10" s="4">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="10" t="s">
+      <c r="I10" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
         <v>51</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -1297,11 +1300,14 @@
       <c r="F11" s="5">
         <v>0.2</v>
       </c>
-      <c r="G11" s="12">
+      <c r="G11" s="6">
         <v>62</v>
       </c>
       <c r="H11" s="4">
         <v>30</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1315,21 +1321,22 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I2"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="54.81640625" customWidth="1"/>
-    <col min="2" max="2" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.1796875" customWidth="1"/>
-    <col min="4" max="4" width="10.1796875" customWidth="1"/>
+    <col min="1" max="1" width="54.83203125" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" customWidth="1"/>
+    <col min="4" max="4" width="10.1640625" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="7" max="7" width="20.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="52.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1348,18 +1355,18 @@
       <c r="F1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="9" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
         <v>21</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -1378,18 +1385,18 @@
         <f>1-D2</f>
         <v>0.4</v>
       </c>
-      <c r="G2" s="12">
+      <c r="G2" s="6">
         <v>112</v>
       </c>
       <c r="H2" s="4">
         <v>30</v>
       </c>
-      <c r="I2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="10" t="s">
+      <c r="I2" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -1408,15 +1415,18 @@
         <f t="shared" ref="F3:F8" si="0">1-D3</f>
         <v>0.44999999999999996</v>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="6">
         <v>112</v>
       </c>
       <c r="H3" s="4">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="10" t="s">
+      <c r="I3" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -1435,15 +1445,18 @@
         <f t="shared" si="0"/>
         <v>0.7</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="6">
         <v>112</v>
       </c>
       <c r="H4" s="4">
         <v>30</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="10" t="s">
+      <c r="I4" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -1452,7 +1465,7 @@
       <c r="C5" s="4">
         <v>0.15</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="4">
         <v>0.5</v>
       </c>
       <c r="E5" s="4">
@@ -1462,15 +1475,18 @@
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="6">
         <v>112</v>
       </c>
       <c r="H5" s="4">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="10" t="s">
+      <c r="I5" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
         <v>24</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -1489,15 +1505,18 @@
         <f t="shared" si="0"/>
         <v>0.7</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="6">
         <v>113</v>
       </c>
       <c r="H6" s="4">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="10" t="s">
+      <c r="I6" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
         <v>25</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -1506,7 +1525,7 @@
       <c r="C7" s="4">
         <v>0.15</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="4">
         <v>0.85</v>
       </c>
       <c r="E7" s="4">
@@ -1516,15 +1535,18 @@
         <f t="shared" si="0"/>
         <v>0.15000000000000002</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="6">
         <v>113</v>
       </c>
       <c r="H7" s="4">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="10" t="s">
+      <c r="I7" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
         <v>47</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -1543,15 +1565,18 @@
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="6">
         <v>112</v>
       </c>
       <c r="H8" s="4">
         <v>30</v>
       </c>
+      <c r="I8" s="4" t="s">
+        <v>113</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
@@ -1562,18 +1587,19 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I2"/>
+      <selection activeCell="I1" sqref="H1:I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="48.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.453125" customWidth="1"/>
-    <col min="7" max="7" width="20.26953125" style="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="52.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1592,18 +1618,18 @@
       <c r="F1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="9" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
         <v>32</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -1622,24 +1648,24 @@
         <f t="shared" ref="F2:F8" si="0">1-D2</f>
         <v>0.31999999999999995</v>
       </c>
-      <c r="G2" s="17">
+      <c r="G2" s="11">
         <v>57</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="4">
         <v>38</v>
       </c>
-      <c r="I2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="3" t="s">
+      <c r="I2" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
         <v>29</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="7">
         <v>0.75</v>
       </c>
       <c r="D3" s="4">
@@ -1652,15 +1678,18 @@
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
-      <c r="G3" s="17">
+      <c r="G3" s="11">
         <v>112</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="4">
         <v>38</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="3" t="s">
+      <c r="I3" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
         <v>28</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -1679,15 +1708,18 @@
         <f t="shared" si="0"/>
         <v>0.7</v>
       </c>
-      <c r="G4" s="17">
+      <c r="G4" s="11">
         <v>112</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="4">
         <v>38</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="3" t="s">
+      <c r="I4" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
         <v>26</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -1696,7 +1728,7 @@
       <c r="C5" s="4">
         <v>0.15</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="4">
         <v>0.65</v>
       </c>
       <c r="E5" s="4">
@@ -1706,15 +1738,18 @@
         <f t="shared" si="0"/>
         <v>0.35</v>
       </c>
-      <c r="G5" s="17">
+      <c r="G5" s="11">
         <v>112</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="4">
         <v>38</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="3" t="s">
+      <c r="I5" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
         <v>27</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -1723,7 +1758,7 @@
       <c r="C6" s="4">
         <v>0.15</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="4">
         <v>0.85</v>
       </c>
       <c r="E6" s="4">
@@ -1733,21 +1768,24 @@
         <f t="shared" si="0"/>
         <v>0.15000000000000002</v>
       </c>
-      <c r="G6" s="17">
+      <c r="G6" s="11">
         <v>112</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="4">
         <v>38</v>
       </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="3" t="s">
+      <c r="I6" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
         <v>48</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="7">
         <v>3.2</v>
       </c>
       <c r="D7" s="4">
@@ -1760,21 +1798,24 @@
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
-      <c r="G7" s="17">
+      <c r="G7" s="11">
         <v>112</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="4">
         <v>38</v>
       </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="3" t="s">
+      <c r="I7" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
         <v>97</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="7">
         <v>3.2</v>
       </c>
       <c r="D8" s="4">
@@ -1787,21 +1828,24 @@
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
-      <c r="G8" s="17">
+      <c r="G8" s="11">
         <v>34</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="4">
         <v>40</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="3" t="s">
+      <c r="I8" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
         <v>94</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="7">
         <v>3.2</v>
       </c>
       <c r="D9" s="4">
@@ -1814,18 +1858,21 @@
         <f>1-D9</f>
         <v>0.4</v>
       </c>
-      <c r="G9" s="17">
+      <c r="G9" s="11">
         <v>73</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="4">
         <v>40</v>
       </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="20"/>
+      <c r="I9" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="14"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
@@ -1835,20 +1882,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="48.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7265625" customWidth="1"/>
-    <col min="3" max="3" width="10.453125" customWidth="1"/>
-    <col min="4" max="4" width="21.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="10.5" customWidth="1"/>
+    <col min="4" max="4" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="52.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1858,131 +1906,145 @@
       <c r="C1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="9" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
         <v>100</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="6">
         <v>2.9</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="6">
         <v>113</v>
       </c>
       <c r="E2" s="4">
         <v>74</v>
       </c>
-      <c r="F2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="3" t="s">
+      <c r="F2" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
         <v>98</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="6">
         <v>0.28000000000000003</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="6">
         <f>D2+44</f>
         <v>157</v>
       </c>
       <c r="E3" s="4">
         <v>74</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="3" t="s">
+      <c r="F3" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
         <v>101</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="6">
         <v>0.25</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="6">
         <v>180</v>
       </c>
       <c r="E4" s="4">
         <v>74</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="3" t="s">
+      <c r="F4" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
         <v>103</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="6">
         <v>2.9</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="6">
         <f>D2+135</f>
         <v>248</v>
       </c>
       <c r="E5" s="4">
         <v>78</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="3" t="s">
+      <c r="F5" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
         <v>104</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="6">
         <v>0.28000000000000003</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="6">
         <f>D3+135</f>
         <v>292</v>
       </c>
       <c r="E6" s="4">
         <v>78</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="3" t="s">
+      <c r="F6" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
         <v>105</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="6">
         <v>0.25</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="6">
         <f>D4+135</f>
         <v>315</v>
       </c>
       <c r="E7" s="4">
         <v>78</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="16"/>
-      <c r="B8" s="15"/>
+      <c r="F7" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B8" s="10"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
@@ -1993,16 +2055,16 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="45.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2014,8 +2076,8 @@
       </c>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -2026,8 +2088,8 @@
       </c>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -2038,8 +2100,8 @@
       </c>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="4" t="s">

</xml_diff>

<commit_message>
renaming all caps variables to lowercase to match all other variables
</commit_message>
<xml_diff>
--- a/cea/databases/CH/assemblies/ENVELOPE.xlsx
+++ b/cea/databases/CH/assemblies/ENVELOPE.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinmo/Documents/Projects/PV/CEA case studies/dummy/inputs/technology/assemblies/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinmo/Documents/GitHub/CityEnergyAnalyst/cea/databases/CH/assemblies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF88A1EE-B6AB-144A-864E-3ADAA09C3669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41F7C203-2C74-3344-9F69-63227A8CD56D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONSTRUCTION" sheetId="7" r:id="rId1"/>
@@ -303,18 +303,6 @@
     <t>SHADING_AS2</t>
   </si>
   <si>
-    <t>GHG_WALL_kgCO2m2</t>
-  </si>
-  <si>
-    <t>GHG_ROOF_kgCO2m2</t>
-  </si>
-  <si>
-    <t>GHG_WIN_kgCO2m2</t>
-  </si>
-  <si>
-    <t>GHG_FLOOR_kgCO2m2</t>
-  </si>
-  <si>
     <t>FLOOR_AS1</t>
   </si>
   <si>
@@ -363,22 +351,34 @@
     <t>FLOOR_AS6</t>
   </si>
   <si>
-    <t>Service_Life_WIN</t>
-  </si>
-  <si>
-    <t>Service_Life_ROOF</t>
-  </si>
-  <si>
-    <t>Service_Life_WALL</t>
-  </si>
-  <si>
-    <t>Service_Life_FLOOR</t>
-  </si>
-  <si>
     <t>Reference</t>
   </si>
   <si>
     <t>Service life reference : https://doi.org/10.1016/j.dib.2021.107062</t>
+  </si>
+  <si>
+    <t>GHG_wall_kgCO2m2</t>
+  </si>
+  <si>
+    <t>Service_Life_wall</t>
+  </si>
+  <si>
+    <t>GHG_floor_kgCO2m2</t>
+  </si>
+  <si>
+    <t>Service_Life_floor</t>
+  </si>
+  <si>
+    <t>GHG_win_kgCO2m2</t>
+  </si>
+  <si>
+    <t>Service_Life_win</t>
+  </si>
+  <si>
+    <t>GHG_roof_kgCO2m2</t>
+  </si>
+  <si>
+    <t>Service_Life_roof</t>
   </si>
 </sst>
 </file>
@@ -815,7 +815,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
@@ -976,7 +976,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1011,13 +1011,13 @@
         <v>52</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -1046,7 +1046,7 @@
         <v>30</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -1075,7 +1075,7 @@
         <v>30</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -1104,7 +1104,7 @@
         <v>30</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -1133,7 +1133,7 @@
         <v>30</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -1162,7 +1162,7 @@
         <v>30</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -1191,7 +1191,7 @@
         <v>30</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -1220,7 +1220,7 @@
         <v>30</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -1249,7 +1249,7 @@
         <v>30</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -1278,7 +1278,7 @@
         <v>30</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -1307,7 +1307,7 @@
         <v>30</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1321,7 +1321,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1356,13 +1356,13 @@
         <v>33</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>89</v>
+        <v>112</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -1392,7 +1392,7 @@
         <v>30</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -1422,7 +1422,7 @@
         <v>30</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -1452,7 +1452,7 @@
         <v>30</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -1482,7 +1482,7 @@
         <v>30</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -1512,7 +1512,7 @@
         <v>30</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -1542,7 +1542,7 @@
         <v>30</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -1572,7 +1572,7 @@
         <v>30</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1587,7 +1587,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="H1:I2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1619,13 +1619,13 @@
         <v>34</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -1655,7 +1655,7 @@
         <v>38</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -1685,7 +1685,7 @@
         <v>38</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -1715,7 +1715,7 @@
         <v>38</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -1745,7 +1745,7 @@
         <v>38</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -1775,7 +1775,7 @@
         <v>38</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -1805,15 +1805,15 @@
         <v>38</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C8" s="7">
         <v>3.2</v>
@@ -1835,15 +1835,15 @@
         <v>40</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C9" s="7">
         <v>3.2</v>
@@ -1865,7 +1865,7 @@
         <v>40</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -1883,7 +1883,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F7"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1907,21 +1907,21 @@
         <v>19</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>91</v>
+        <v>108</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C2" s="6">
         <v>2.9</v>
@@ -1933,15 +1933,15 @@
         <v>74</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C3" s="6">
         <v>0.28000000000000003</v>
@@ -1954,15 +1954,15 @@
         <v>74</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C4" s="6">
         <v>0.25</v>
@@ -1974,15 +1974,15 @@
         <v>74</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C5" s="6">
         <v>2.9</v>
@@ -1995,15 +1995,15 @@
         <v>78</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C6" s="6">
         <v>0.28000000000000003</v>
@@ -2016,15 +2016,15 @@
         <v>78</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C7" s="6">
         <v>0.25</v>
@@ -2037,7 +2037,7 @@
         <v>78</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -2054,8 +2054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update embodied module final version
</commit_message>
<xml_diff>
--- a/cea/databases/CH/assemblies/ENVELOPE.xlsx
+++ b/cea/databases/CH/assemblies/ENVELOPE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmeshkin\Documents\GitHub\CityEnergyAnalyst\cea\databases\SG\assemblies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmeshkin\Documents\GitHub\CityEnergyAnalyst\cea\databases\CH\assemblies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{610468E6-D4FE-45AD-B8D6-65815784530B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95057C72-AB98-4CA8-BE85-145C14ECCE18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONSTRUCTION" sheetId="7" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="156">
   <si>
     <t>Description</t>
   </si>
@@ -351,27 +351,15 @@
     <t>FLOOR_AS6</t>
   </si>
   <si>
-    <t>GHG_wall_kgCO2m2</t>
-  </si>
-  <si>
     <t>Service_Life_wall</t>
   </si>
   <si>
-    <t>GHG_floor_kgCO2m2</t>
-  </si>
-  <si>
     <t>Service_Life_floor</t>
   </si>
   <si>
-    <t>GHG_win_kgCO2m2</t>
-  </si>
-  <si>
     <t>Service_Life_win</t>
   </si>
   <si>
-    <t>GHG_roof_kgCO2m2</t>
-  </si>
-  <si>
     <t>Service_Life_roof</t>
   </si>
   <si>
@@ -379,6 +367,144 @@
   </si>
   <si>
     <t>Reference Service life</t>
+  </si>
+  <si>
+    <t>GWP_fossil_floor_kgCO2m2</t>
+  </si>
+  <si>
+    <t>GWP_biogenic_floor_kgCO2m2</t>
+  </si>
+  <si>
+    <t>NoStructur basement concrete - new - conventional - sia 2024</t>
+  </si>
+  <si>
+    <t>NoStructur basement concrete - new - low carbon - sia 2024</t>
+  </si>
+  <si>
+    <t>NoStructur basement concrete - new - negative - sia 2024</t>
+  </si>
+  <si>
+    <t>NoStructur floor concrete - new - conventional</t>
+  </si>
+  <si>
+    <t>NoStructur floor concrete - new - low carbon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NoStructur floor concrete - new - negative </t>
+  </si>
+  <si>
+    <t>NoStructur external wall - new- conventional - sia 2024</t>
+  </si>
+  <si>
+    <t>NoStructur external wall - new- low carbon- sia 2024</t>
+  </si>
+  <si>
+    <t>NoStructur external wall - new- negative carbon- sia 2024</t>
+  </si>
+  <si>
+    <t>NoStruct Flat roof - new- conventional - sia 2024</t>
+  </si>
+  <si>
+    <t>NoStruct Flat roof - new- low carbon- sia 2024</t>
+  </si>
+  <si>
+    <t>NoStruct Flat roof - new- negative carbon- sia 2024</t>
+  </si>
+  <si>
+    <t>Light construction - new</t>
+  </si>
+  <si>
+    <t>CONSTRUCTION_AS4</t>
+  </si>
+  <si>
+    <t>Medium construction -new</t>
+  </si>
+  <si>
+    <t>CONSTRUCTION_AS5</t>
+  </si>
+  <si>
+    <t>Tracking Construction Material over Space and Time: Prospective and Geo-referenced Modeling of Building Stocks and Construction Material Flows; KBOB</t>
+  </si>
+  <si>
+    <t>GWP_fossil_cons_kgCO2m2</t>
+  </si>
+  <si>
+    <t>GWP_biogenic_cons_kgCO2m2</t>
+  </si>
+  <si>
+    <t>Service_Life_cons</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>No retrofit</t>
+  </si>
+  <si>
+    <t>WINDOW_NoRet</t>
+  </si>
+  <si>
+    <t>NoRotrofit</t>
+  </si>
+  <si>
+    <t>ROOF_NoRet</t>
+  </si>
+  <si>
+    <t>WALL_NoRet</t>
+  </si>
+  <si>
+    <t>FLOOR_NoRet</t>
+  </si>
+  <si>
+    <t>GWP_fossil_wall_kgCO2m2</t>
+  </si>
+  <si>
+    <t>GWP_biogenic_wall_kgCO2m2</t>
+  </si>
+  <si>
+    <t>GWP_fossil_roof_kgCO2m2</t>
+  </si>
+  <si>
+    <t>GWP_biogenic_roof_kgCO2m2</t>
+  </si>
+  <si>
+    <t>ROOF_AS8_C</t>
+  </si>
+  <si>
+    <t>ROOF_AS8_L</t>
+  </si>
+  <si>
+    <t>ROOF_AS8_N</t>
+  </si>
+  <si>
+    <t>GWP_win_kgCO2m2</t>
+  </si>
+  <si>
+    <t>WALL_AS9_C</t>
+  </si>
+  <si>
+    <t>WALL_AS9_L</t>
+  </si>
+  <si>
+    <t>WALL_AS9_N</t>
+  </si>
+  <si>
+    <t>FLOOR_AS7_C</t>
+  </si>
+  <si>
+    <t>FLOOR_AS7_L</t>
+  </si>
+  <si>
+    <t>FLOOR_AS7_N</t>
+  </si>
+  <si>
+    <t>FLOOR_AS8_C</t>
+  </si>
+  <si>
+    <t>FLOOR_AS8_L</t>
+  </si>
+  <si>
+    <t>FLOOR_AS8_N</t>
   </si>
 </sst>
 </file>
@@ -388,7 +514,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -421,15 +547,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <i/>
-      <sz val="10"/>
-      <color rgb="FF8C8C8C"/>
-      <name val="Arial Unicode MS"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -448,8 +567,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9900"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -483,12 +608,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -517,20 +655,46 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -813,20 +977,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="22.453125" customWidth="1"/>
     <col min="2" max="2" width="19.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -836,8 +1000,20 @@
       <c r="C1" s="3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>37</v>
       </c>
@@ -847,8 +1023,18 @@
       <c r="C2" s="4">
         <v>110000</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" s="14">
+        <v>0</v>
+      </c>
+      <c r="E2" s="14">
+        <v>0</v>
+      </c>
+      <c r="F2" s="14">
+        <v>60</v>
+      </c>
+      <c r="G2" s="14"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>38</v>
       </c>
@@ -858,8 +1044,18 @@
       <c r="C3" s="4">
         <v>165000</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" s="14">
+        <v>0</v>
+      </c>
+      <c r="E3" s="14">
+        <v>0</v>
+      </c>
+      <c r="F3" s="14">
+        <v>60</v>
+      </c>
+      <c r="G3" s="14"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>36</v>
       </c>
@@ -868,6 +1064,62 @@
       </c>
       <c r="C4" s="4">
         <v>300000</v>
+      </c>
+      <c r="D4" s="14">
+        <v>0</v>
+      </c>
+      <c r="E4" s="14">
+        <v>0</v>
+      </c>
+      <c r="F4" s="14">
+        <v>60</v>
+      </c>
+      <c r="G4" s="14"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C5" s="4">
+        <v>110000</v>
+      </c>
+      <c r="D5" s="19">
+        <v>6.9</v>
+      </c>
+      <c r="E5" s="19">
+        <v>-65.5</v>
+      </c>
+      <c r="F5" s="14">
+        <v>60</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C6" s="4">
+        <v>165000</v>
+      </c>
+      <c r="D6" s="19">
+        <v>82.9</v>
+      </c>
+      <c r="E6" s="19">
+        <v>0</v>
+      </c>
+      <c r="F6" s="14">
+        <v>60</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -883,13 +1135,13 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17.6328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -900,7 +1152,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>43</v>
       </c>
@@ -911,7 +1163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>39</v>
       </c>
@@ -922,7 +1174,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>44</v>
       </c>
@@ -933,7 +1185,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>42</v>
       </c>
@@ -944,7 +1196,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>40</v>
       </c>
@@ -955,7 +1207,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
         <v>41</v>
       </c>
@@ -973,13 +1225,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="51.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
@@ -991,7 +1243,7 @@
     <col min="9" max="9" width="52.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1011,16 +1263,16 @@
         <v>52</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>108</v>
+        <v>146</v>
       </c>
       <c r="H1" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="I1" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="I1" s="9" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>5</v>
       </c>
@@ -1046,10 +1298,10 @@
         <v>30</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>31</v>
       </c>
@@ -1075,10 +1327,10 @@
         <v>30</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>30</v>
       </c>
@@ -1104,10 +1356,10 @@
         <v>30</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>6</v>
       </c>
@@ -1133,10 +1385,10 @@
         <v>30</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>46</v>
       </c>
@@ -1162,10 +1414,10 @@
         <v>30</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
         <v>7</v>
       </c>
@@ -1191,10 +1443,10 @@
         <v>30</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
         <v>8</v>
       </c>
@@ -1220,10 +1472,10 @@
         <v>30</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
         <v>49</v>
       </c>
@@ -1249,10 +1501,10 @@
         <v>30</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
         <v>50</v>
       </c>
@@ -1278,10 +1530,10 @@
         <v>30</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
         <v>51</v>
       </c>
@@ -1307,8 +1559,35 @@
         <v>30</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>112</v>
-      </c>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="C12" s="20">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D12" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="E12" s="21">
+        <v>0.89</v>
+      </c>
+      <c r="F12" s="21">
+        <v>0.2</v>
+      </c>
+      <c r="G12" s="20">
+        <v>0</v>
+      </c>
+      <c r="H12" s="20">
+        <v>60</v>
+      </c>
+      <c r="I12" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1318,25 +1597,26 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I2"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="54.81640625" customWidth="1"/>
-    <col min="2" max="2" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.1796875" customWidth="1"/>
     <col min="4" max="4" width="10.1796875" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
     <col min="7" max="7" width="20.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="52.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.36328125" customWidth="1"/>
+    <col min="9" max="9" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="52.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1356,16 +1636,19 @@
         <v>33</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>110</v>
+        <v>141</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>111</v>
+        <v>142</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+        <v>107</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>21</v>
       </c>
@@ -1388,14 +1671,17 @@
       <c r="G2" s="6">
         <v>112</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="6">
+        <v>0</v>
+      </c>
+      <c r="I2" s="4">
         <v>60</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="J2" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>20</v>
       </c>
@@ -1418,14 +1704,17 @@
       <c r="G3" s="6">
         <v>112</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="6">
+        <v>0</v>
+      </c>
+      <c r="I3" s="4">
         <v>60</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="J3" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>23</v>
       </c>
@@ -1448,14 +1737,17 @@
       <c r="G4" s="6">
         <v>112</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="6">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4">
         <v>60</v>
       </c>
-      <c r="I4" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="J4" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>22</v>
       </c>
@@ -1478,14 +1770,17 @@
       <c r="G5" s="6">
         <v>112</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="6">
+        <v>0</v>
+      </c>
+      <c r="I5" s="4">
         <v>60</v>
       </c>
-      <c r="I5" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="J5" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>24</v>
       </c>
@@ -1508,14 +1803,17 @@
       <c r="G6" s="6">
         <v>113</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="6">
+        <v>0</v>
+      </c>
+      <c r="I6" s="4">
         <v>60</v>
       </c>
-      <c r="I6" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="J6" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
         <v>25</v>
       </c>
@@ -1538,42 +1836,169 @@
       <c r="G7" s="6">
         <v>113</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="6">
+        <v>0</v>
+      </c>
+      <c r="I7" s="4">
         <v>60</v>
       </c>
-      <c r="I7" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="8" t="s">
+      <c r="J7" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="13">
         <v>0.6</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="13">
         <v>0.6</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="13">
         <v>0.94</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="13">
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
       <c r="G8" s="6">
         <v>112</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="6">
+        <v>0</v>
+      </c>
+      <c r="I8" s="13">
         <v>60</v>
       </c>
-      <c r="I8" s="4" t="s">
-        <v>112</v>
-      </c>
+      <c r="J8" s="13" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0.94</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="G9" s="4">
+        <v>140</v>
+      </c>
+      <c r="H9" s="4">
+        <v>0</v>
+      </c>
+      <c r="I9" s="4">
+        <v>60</v>
+      </c>
+      <c r="J9" s="4"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0.94</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="G10" s="4">
+        <v>70</v>
+      </c>
+      <c r="H10" s="4">
+        <v>-17</v>
+      </c>
+      <c r="I10" s="4">
+        <v>60</v>
+      </c>
+      <c r="J10" s="4"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0.94</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="G11" s="4">
+        <v>108</v>
+      </c>
+      <c r="H11" s="4">
+        <v>-95</v>
+      </c>
+      <c r="I11" s="4">
+        <v>60</v>
+      </c>
+      <c r="J11" s="4"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="C12" s="20">
+        <v>0.6</v>
+      </c>
+      <c r="D12" s="20">
+        <v>0.6</v>
+      </c>
+      <c r="E12" s="20">
+        <v>0.94</v>
+      </c>
+      <c r="F12" s="20">
+        <f t="shared" ref="F12" si="1">1-D12</f>
+        <v>0.4</v>
+      </c>
+      <c r="G12" s="20">
+        <v>0</v>
+      </c>
+      <c r="H12" s="20">
+        <v>0</v>
+      </c>
+      <c r="I12" s="20">
+        <v>60</v>
+      </c>
+      <c r="J12" s="20"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -1584,22 +2009,23 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="48.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.453125" customWidth="1"/>
-    <col min="7" max="7" width="20.36328125" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="52.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.36328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.36328125" style="11" customWidth="1"/>
+    <col min="9" max="9" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="52.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1618,17 +2044,20 @@
       <c r="F1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="I1" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="H1" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>32</v>
       </c>
@@ -1648,17 +2077,20 @@
         <f t="shared" ref="F2:F8" si="0">1-D2</f>
         <v>0.31999999999999995</v>
       </c>
-      <c r="G2" s="11">
+      <c r="G2" s="10">
         <v>57</v>
       </c>
-      <c r="H2" s="4">
-        <v>30</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="H2" s="10">
+        <v>0</v>
+      </c>
+      <c r="I2" s="4">
+        <v>30</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>29</v>
       </c>
@@ -1678,17 +2110,20 @@
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
-      <c r="G3" s="11">
+      <c r="G3" s="10">
         <v>112</v>
       </c>
-      <c r="H3" s="4">
-        <v>30</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="H3" s="10">
+        <v>0</v>
+      </c>
+      <c r="I3" s="4">
+        <v>30</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>28</v>
       </c>
@@ -1708,17 +2143,20 @@
         <f t="shared" si="0"/>
         <v>0.7</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="10">
         <v>112</v>
       </c>
-      <c r="H4" s="4">
-        <v>30</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="H4" s="10">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4">
+        <v>30</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>26</v>
       </c>
@@ -1738,17 +2176,20 @@
         <f t="shared" si="0"/>
         <v>0.35</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="10">
         <v>112</v>
       </c>
-      <c r="H5" s="4">
-        <v>30</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="H5" s="10">
+        <v>0</v>
+      </c>
+      <c r="I5" s="4">
+        <v>30</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>27</v>
       </c>
@@ -1768,17 +2209,20 @@
         <f t="shared" si="0"/>
         <v>0.15000000000000002</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="10">
         <v>112</v>
       </c>
-      <c r="H6" s="4">
-        <v>30</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="H6" s="10">
+        <v>0</v>
+      </c>
+      <c r="I6" s="4">
+        <v>30</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
         <v>48</v>
       </c>
@@ -1798,17 +2242,20 @@
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="10">
         <v>112</v>
       </c>
-      <c r="H7" s="4">
-        <v>30</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="H7" s="10">
+        <v>0</v>
+      </c>
+      <c r="I7" s="4">
+        <v>30</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
         <v>93</v>
       </c>
@@ -1828,48 +2275,179 @@
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="10">
         <v>34</v>
       </c>
-      <c r="H8" s="4">
-        <v>30</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="8" t="s">
+      <c r="H8" s="10">
+        <v>0</v>
+      </c>
+      <c r="I8" s="4">
+        <v>30</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="16">
         <v>3.2</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="13">
         <v>0.6</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="13">
         <v>0.95</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="13">
         <f>1-D9</f>
         <v>0.4</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="17">
         <v>73</v>
       </c>
-      <c r="H9" s="4">
-        <v>30</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="14"/>
+      <c r="H9" s="17">
+        <v>0</v>
+      </c>
+      <c r="I9" s="13">
+        <v>30</v>
+      </c>
+      <c r="J9" s="13" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0.84</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="G10" s="18">
+        <v>102</v>
+      </c>
+      <c r="H10" s="18">
+        <v>0</v>
+      </c>
+      <c r="I10" s="13">
+        <v>30</v>
+      </c>
+      <c r="J10" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0.84</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="G11" s="18">
+        <v>30</v>
+      </c>
+      <c r="H11" s="18">
+        <v>-16</v>
+      </c>
+      <c r="I11" s="13">
+        <v>30</v>
+      </c>
+      <c r="J11" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="E12" s="4">
+        <v>0.84</v>
+      </c>
+      <c r="F12" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="G12" s="18">
+        <v>66</v>
+      </c>
+      <c r="H12" s="18">
+        <v>-90</v>
+      </c>
+      <c r="I12" s="13">
+        <v>30</v>
+      </c>
+      <c r="J12" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="C13" s="20">
+        <v>3.2</v>
+      </c>
+      <c r="D13" s="20">
+        <v>0.6</v>
+      </c>
+      <c r="E13" s="20">
+        <v>0.95</v>
+      </c>
+      <c r="F13" s="20">
+        <v>0.4</v>
+      </c>
+      <c r="G13" s="20">
+        <v>0</v>
+      </c>
+      <c r="H13" s="20">
+        <v>0</v>
+      </c>
+      <c r="I13" s="20">
+        <v>60</v>
+      </c>
+      <c r="J13" s="20">
+        <v>60</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -1880,23 +2458,24 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="48.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6328125" customWidth="1"/>
+    <col min="2" max="2" width="15.54296875" customWidth="1"/>
     <col min="3" max="3" width="10.453125" customWidth="1"/>
     <col min="4" max="4" width="21.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="52.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.453125" customWidth="1"/>
+    <col min="6" max="6" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="52.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1907,16 +2486,19 @@
         <v>19</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+        <v>105</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>96</v>
       </c>
@@ -1929,14 +2511,17 @@
       <c r="D2" s="6">
         <v>113</v>
       </c>
-      <c r="E2" s="4">
-        <v>30</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="E2" s="6">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4">
+        <v>30</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>94</v>
       </c>
@@ -1950,14 +2535,17 @@
         <f>D2+44</f>
         <v>157</v>
       </c>
-      <c r="E3" s="4">
-        <v>30</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="E3" s="6">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>30</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>97</v>
       </c>
@@ -1970,14 +2558,17 @@
       <c r="D4" s="6">
         <v>180</v>
       </c>
-      <c r="E4" s="4">
-        <v>30</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="E4" s="6">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>30</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>99</v>
       </c>
@@ -1991,14 +2582,17 @@
         <f>D2+135</f>
         <v>248</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="6">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4">
         <v>60</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>100</v>
       </c>
@@ -2012,36 +2606,186 @@
         <f>D3+135</f>
         <v>292</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="6">
+        <v>0</v>
+      </c>
+      <c r="F6" s="4">
         <v>60</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="8" t="s">
+      <c r="G6" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="12">
         <v>0.25</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="12">
         <f>D4+135</f>
         <v>315</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="12">
+        <v>0</v>
+      </c>
+      <c r="F7" s="13">
         <v>60</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="G7" s="13" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="8" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="B8" s="10"/>
+      <c r="B8" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="D8" s="4">
+        <v>112</v>
+      </c>
+      <c r="E8" s="4">
+        <v>-60</v>
+      </c>
+      <c r="F8" s="4">
+        <v>60</v>
+      </c>
+      <c r="G8" s="14"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="D9" s="4">
+        <v>43</v>
+      </c>
+      <c r="E9" s="4">
+        <v>-77</v>
+      </c>
+      <c r="F9" s="4">
+        <v>60</v>
+      </c>
+      <c r="G9" s="14"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="D10" s="4">
+        <v>79</v>
+      </c>
+      <c r="E10" s="4">
+        <v>-150</v>
+      </c>
+      <c r="F10" s="4">
+        <v>60</v>
+      </c>
+      <c r="G10" s="14"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0.17</v>
+      </c>
+      <c r="D11" s="4">
+        <v>81</v>
+      </c>
+      <c r="E11" s="4">
+        <v>-60</v>
+      </c>
+      <c r="F11" s="4">
+        <v>30</v>
+      </c>
+      <c r="G11" s="14"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0.17</v>
+      </c>
+      <c r="D12" s="4">
+        <v>41</v>
+      </c>
+      <c r="E12" s="4">
+        <v>-69</v>
+      </c>
+      <c r="F12" s="4">
+        <v>30</v>
+      </c>
+      <c r="G12" s="14"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C13" s="4">
+        <v>0.17</v>
+      </c>
+      <c r="D13" s="4">
+        <v>62</v>
+      </c>
+      <c r="E13" s="4">
+        <v>-111</v>
+      </c>
+      <c r="F13" s="4">
+        <v>30</v>
+      </c>
+      <c r="G13" s="14"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="C14" s="20">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="D14" s="20">
+        <v>0</v>
+      </c>
+      <c r="E14" s="20">
+        <v>0</v>
+      </c>
+      <c r="F14" s="20">
+        <v>60</v>
+      </c>
+      <c r="G14" s="14"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -2058,13 +2802,13 @@
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="45.36328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2076,7 +2820,7 @@
       </c>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
@@ -2088,7 +2832,7 @@
       </c>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>15</v>
       </c>
@@ -2100,7 +2844,7 @@
       </c>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>10</v>
       </c>

</xml_diff>